<commit_message>
Changed TT by Thushy
</commit_message>
<xml_diff>
--- a/TimeTable.xlsx
+++ b/TimeTable.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThusyStudyPath\Path\ThusyStudies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Notes\ThusyStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B954F5E-7D4E-4110-BD3B-3CDDC885B8AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{B8D059CA-6E6D-45E3-A2AA-0A0F103055A6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -603,7 +602,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1068,11 +1067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB9EAB5-D0D3-4BF9-8A8F-ABF57B751082}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1121,11 +1120,11 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2">
         <f>D8+D21+D29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <f>E8+E21+E29</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
         <v>184</v>
@@ -1138,22 +1137,25 @@
       <c r="C8" s="5"/>
       <c r="D8" s="3">
         <f>SUM(D9:D20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4">
         <f>SUM(E9:E20)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>6</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>9</v>
       </c>
@@ -1201,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>10</v>
       </c>
@@ -1209,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>12</v>
       </c>
@@ -1225,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -1233,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
class and objects notes added
</commit_message>
<xml_diff>
--- a/TimeTable.xlsx
+++ b/TimeTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThusyStudyPath\Path\ThusyStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14A7EAB-3939-44C6-A371-CD81C5230377}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C58EE-26ED-43C0-862B-8A5D99019F43}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="224">
   <si>
     <t>Module</t>
   </si>
@@ -696,6 +696,12 @@
   </si>
   <si>
     <t>methods</t>
+  </si>
+  <si>
+    <t>Access Modifiers</t>
+  </si>
+  <si>
+    <t>Methods</t>
   </si>
 </sst>
 </file>
@@ -1414,78 +1420,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A8C831-C4F6-4DE4-BDF3-BFAB179B5753}">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>195</v>
       </c>
       <c r="C3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>202</v>
       </c>
@@ -1499,17 +1538,17 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>205</v>
       </c>

</xml_diff>